<commit_message>
Add bat and update time
</commit_message>
<xml_diff>
--- a/IDCM Compare.xlsx
+++ b/IDCM Compare.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XX\Projects\ccxt\ticker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\XX\Projects\ccxt\price_compare\IDCM_Compare\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="26">
   <si>
     <t>USDT:CNY 汇率</t>
   </si>
@@ -103,15 +103,20 @@
   </si>
   <si>
     <t>收到 VHKD</t>
+  </si>
+  <si>
+    <t>更新时间</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="179" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -190,7 +195,7 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +219,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="百分比" xfId="2" builtinId="5"/>
@@ -246,62 +253,67 @@
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2">
+            <v>1526350746056</v>
+          </cell>
+        </row>
         <row r="3">
           <cell r="B3">
-            <v>8385.35</v>
+            <v>8673.3700000000008</v>
           </cell>
           <cell r="C3">
-            <v>8380.8914999999997</v>
+            <v>8669.6635999999999</v>
           </cell>
           <cell r="D3">
-            <v>8368.4500000000007</v>
+            <v>8664.42</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>8387.9</v>
+            <v>8679.86</v>
           </cell>
           <cell r="C4">
-            <v>8396.8011999999999</v>
+            <v>8687.1563999999998</v>
           </cell>
           <cell r="D4">
-            <v>8385.3700000000008</v>
+            <v>8676.48</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="B3">
-            <v>705.97</v>
+            <v>726.21</v>
           </cell>
           <cell r="C3">
-            <v>705.67809999999997</v>
+            <v>725.86</v>
           </cell>
           <cell r="D3">
-            <v>704.31</v>
+            <v>726.68</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>706.8</v>
+            <v>726.27</v>
           </cell>
           <cell r="C4">
-            <v>706.09209999999996</v>
+            <v>726.94200000000001</v>
           </cell>
           <cell r="D4">
-            <v>706.1</v>
+            <v>727.34</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2">
         <row r="3">
           <cell r="B3">
-            <v>6.57</v>
+            <v>6.5</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>6.58</v>
+            <v>6.51</v>
           </cell>
         </row>
       </sheetData>
@@ -313,7 +325,7 @@
         </row>
         <row r="4">
           <cell r="B4">
-            <v>0.82769999999999999</v>
+            <v>0.82879999999999998</v>
           </cell>
         </row>
       </sheetData>
@@ -621,16 +633,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.1328125" customWidth="1"/>
-    <col min="2" max="6" width="28.1328125" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="15">
+        <f>([1]btc_ticker_price!$B$2/1000+8*3600)/86400+70*365+19</f>
+        <v>43235.429931203704</v>
+      </c>
+      <c r="C1" s="16">
+        <f>([1]btc_ticker_price!$B$2/1000+8*3600)/86400+70*365+19</f>
+        <v>43235.429931203704</v>
+      </c>
+    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>12</v>
@@ -660,19 +689,19 @@
       </c>
       <c r="C5" s="11">
         <f>[1]usdt_c2c_price!$B$4</f>
-        <v>6.58</v>
+        <v>6.51</v>
       </c>
       <c r="D5" s="2">
         <f>B5/C5</f>
-        <v>15197.568389057751</v>
+        <v>15360.983102918588</v>
       </c>
       <c r="E5" s="11">
         <f>[1]btc_ticker_price!$B$4</f>
-        <v>8387.9</v>
+        <v>8679.86</v>
       </c>
       <c r="F5" s="8">
         <f>D5/E5</f>
-        <v>1.8118442505344308</v>
+        <v>1.7697270581459363</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -691,11 +720,11 @@
       </c>
       <c r="E6" s="11">
         <f>[1]btc_ticker_price!$C$4</f>
-        <v>8396.8011999999999</v>
+        <v>8687.1563999999998</v>
       </c>
       <c r="F6" s="8">
         <f t="shared" ref="F6:F10" si="1">D6/E6</f>
-        <v>1.7989874740953593</v>
+        <v>1.7388590104431505</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -714,11 +743,11 @@
       </c>
       <c r="E7" s="11">
         <f>[1]btc_ticker_price!$D$4</f>
-        <v>8385.3700000000008</v>
+        <v>8676.48</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="1"/>
-        <v>1.8030741165238211</v>
+        <v>1.7425780506006301</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -755,18 +784,18 @@
       </c>
       <c r="C10" s="11">
         <f>[1]vhkd_c2c_price!$B$4</f>
-        <v>0.82769999999999999</v>
+        <v>0.82879999999999998</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>120816.72103419113</v>
+        <v>120656.37065637067</v>
       </c>
       <c r="E10" s="12">
         <v>66033</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
-        <v>1.8296415585266628</v>
+        <v>1.8272132215160701</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
@@ -775,7 +804,7 @@
       </c>
       <c r="F12" s="5">
         <f>(F10/(AVERAGE(F5,F6,F7))-1)</f>
-        <v>1.3856693601156378E-2</v>
+        <v>4.3890371758949609E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
@@ -807,19 +836,19 @@
       </c>
       <c r="C18" s="11">
         <f>[1]btc_ticker_price!$B$3</f>
-        <v>8385.35</v>
+        <v>8673.3700000000008</v>
       </c>
       <c r="D18" s="2">
         <f>C18*B18</f>
-        <v>16770.7</v>
+        <v>17346.740000000002</v>
       </c>
       <c r="E18" s="14">
         <f>[1]usdt_c2c_price!$B$3</f>
-        <v>6.57</v>
+        <v>6.5</v>
       </c>
       <c r="F18" s="10">
         <f>D18*E18</f>
-        <v>110183.49900000001</v>
+        <v>112753.81000000001</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -831,18 +860,18 @@
       </c>
       <c r="C19" s="11">
         <f>[1]btc_ticker_price!$C$3</f>
-        <v>8380.8914999999997</v>
+        <v>8669.6635999999999</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ref="D19:D20" si="2">C19*B19</f>
-        <v>16761.782999999999</v>
+        <v>17339.3272</v>
       </c>
       <c r="E19" s="13">
         <v>6.61</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" ref="F19:F20" si="3">D19*E19</f>
-        <v>110795.38563</v>
+        <v>114612.95279200001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -854,18 +883,18 @@
       </c>
       <c r="C20" s="11">
         <f>[1]btc_ticker_price!$D$3</f>
-        <v>8368.4500000000007</v>
+        <v>8664.42</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="2"/>
-        <v>16736.900000000001</v>
+        <v>17328.84</v>
       </c>
       <c r="E20" s="13">
         <v>6.61</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="3"/>
-        <v>110630.90900000001</v>
+        <v>114543.6324</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -929,7 +958,7 @@
       </c>
       <c r="F25" s="5">
         <f>-(F23/(AVERAGE(F18,F19,F20))-1)</f>
-        <v>2.0287198265037776E-2</v>
+        <v>4.9802624990205158E-2</v>
       </c>
     </row>
   </sheetData>
@@ -943,12 +972,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.1328125" customWidth="1"/>
-    <col min="2" max="6" width="28.1328125" customWidth="1"/>
+    <col min="1" max="1" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
@@ -980,19 +1015,19 @@
       </c>
       <c r="C5" s="11">
         <f>[1]usdt_c2c_price!$B$4</f>
-        <v>6.58</v>
+        <v>6.51</v>
       </c>
       <c r="D5" s="2">
         <f>B5/C5</f>
-        <v>15197.568389057751</v>
+        <v>15360.983102918588</v>
       </c>
       <c r="E5" s="11">
         <f>[1]eth_ticker_price!$B$4</f>
-        <v>706.8</v>
+        <v>726.27</v>
       </c>
       <c r="F5" s="8">
         <f>D5/E5</f>
-        <v>21.501936034320533</v>
+        <v>21.150513036361943</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.4">
@@ -1011,11 +1046,11 @@
       </c>
       <c r="E6" s="11">
         <f>[1]eth_ticker_price!$C$4</f>
-        <v>706.09209999999996</v>
+        <v>726.94200000000001</v>
       </c>
       <c r="F6" s="8">
         <f t="shared" ref="F6:F10" si="1">D6/E6</f>
-        <v>21.393441707206303</v>
+        <v>20.779842382568187</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.4">
@@ -1034,11 +1069,11 @@
       </c>
       <c r="E7" s="11">
         <f>[1]eth_ticker_price!$D$4</f>
-        <v>706.1</v>
+        <v>727.34</v>
       </c>
       <c r="F7" s="8">
         <f t="shared" si="1"/>
-        <v>21.412609551728302</v>
+        <v>20.787312129781608</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.4">
@@ -1075,18 +1110,18 @@
       </c>
       <c r="C10" s="11">
         <f>[1]vhkd_c2c_price!$B$4</f>
-        <v>0.82769999999999999</v>
+        <v>0.82879999999999998</v>
       </c>
       <c r="D10" s="7">
         <f t="shared" si="0"/>
-        <v>120816.72103419113</v>
+        <v>120656.37065637067</v>
       </c>
       <c r="E10" s="12">
         <v>66033</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="1"/>
-        <v>1.8296415585266628</v>
+        <v>1.8272132215160701</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.4">
@@ -1095,7 +1130,7 @@
       </c>
       <c r="F12" s="5">
         <f>(F10/(AVERAGE(F5,F6,F7))-1)</f>
-        <v>-0.91464629968048017</v>
+        <v>-0.91259815808215905</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.4">
@@ -1127,19 +1162,19 @@
       </c>
       <c r="C18" s="11">
         <f>[1]eth_ticker_price!$B$3</f>
-        <v>705.97</v>
+        <v>726.21</v>
       </c>
       <c r="D18" s="2">
         <f>C18*B18</f>
-        <v>1411.94</v>
+        <v>1452.42</v>
       </c>
       <c r="E18" s="14">
         <f>[1]usdt_c2c_price!$B$3</f>
-        <v>6.57</v>
+        <v>6.5</v>
       </c>
       <c r="F18" s="10">
         <f>D18*E18</f>
-        <v>9276.4458000000013</v>
+        <v>9440.73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.4">
@@ -1151,18 +1186,18 @@
       </c>
       <c r="C19" s="11">
         <f>[1]eth_ticker_price!$C$3</f>
-        <v>705.67809999999997</v>
+        <v>725.86</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" ref="D19:D20" si="2">C19*B19</f>
-        <v>1411.3561999999999</v>
+        <v>1451.72</v>
       </c>
       <c r="E19" s="13">
         <v>6.61</v>
       </c>
       <c r="F19" s="10">
         <f t="shared" ref="F19:F20" si="3">D19*E19</f>
-        <v>9329.0644819999998</v>
+        <v>9595.869200000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.4">
@@ -1174,18 +1209,18 @@
       </c>
       <c r="C20" s="11">
         <f>[1]eth_ticker_price!$D$3</f>
-        <v>704.31</v>
+        <v>726.68</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="2"/>
-        <v>1408.62</v>
+        <v>1453.36</v>
       </c>
       <c r="E20" s="13">
         <v>6.61</v>
       </c>
       <c r="F20" s="10">
         <f t="shared" si="3"/>
-        <v>9310.9781999999996</v>
+        <v>9606.7096000000001</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.4">
@@ -1249,7 +1284,7 @@
       </c>
       <c r="F25" s="5">
         <f>-(F23/(AVERAGE(F18,F19,F20))-1)</f>
-        <v>-10.637651354663667</v>
+        <v>-10.342347431592819</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
link USDT price of ETH sheet to BTC sheet
</commit_message>
<xml_diff>
--- a/IDCM Compare.xlsx
+++ b/IDCM Compare.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="BTC" sheetId="1" r:id="rId1"/>
@@ -131,13 +131,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="0.000000"/>
     <numFmt numFmtId="178" formatCode="0.0000"/>
-    <numFmt numFmtId="182" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="183" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="179" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -292,7 +291,7 @@
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -352,7 +351,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -520,82 +519,82 @@
       <sheetData sheetId="0">
         <row r="2">
           <cell r="B2">
-            <v>1526363554540</v>
+            <v>1526550039052</v>
           </cell>
         </row>
         <row r="3">
           <cell r="B3">
-            <v>8717.17</v>
+            <v>8283.7199999999993</v>
           </cell>
           <cell r="C3">
-            <v>8718.7561999999998</v>
+            <v>8287.5108</v>
           </cell>
           <cell r="D3">
-            <v>8701.2999999999993</v>
+            <v>8300.7199999999993</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>8717.2900000000009</v>
+            <v>8285.5400000000009</v>
           </cell>
           <cell r="C4">
-            <v>8722.9490000000005</v>
+            <v>8292.8068999999996</v>
           </cell>
           <cell r="D4">
-            <v>8711</v>
+            <v>8301.02</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="3">
           <cell r="B3">
-            <v>733</v>
+            <v>704.1</v>
           </cell>
           <cell r="C3">
-            <v>732.327</v>
+            <v>702.86779999999999</v>
           </cell>
           <cell r="D3">
-            <v>732.37</v>
+            <v>703.72</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>733.01</v>
+            <v>704.38</v>
           </cell>
           <cell r="C4">
-            <v>733.7799</v>
+            <v>703.81910000000005</v>
           </cell>
           <cell r="D4">
-            <v>734.15</v>
+            <v>704.71</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2">
         <row r="3">
           <cell r="B3">
-            <v>6.48</v>
+            <v>6.49</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>6.49</v>
+            <v>6.5</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="3">
         <row r="3">
           <cell r="B3">
-            <v>0.80620000000000003</v>
+            <v>0.80769999999999997</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>0.82199999999999995</v>
+            <v>0.82299999999999995</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -916,11 +915,11 @@
       </c>
       <c r="B1" s="32">
         <f>([1]btc_ticker_price!$B$2/1000+8*3600)/86400+70*365+19</f>
-        <v>43235.578177546297</v>
+        <v>43237.736563101847</v>
       </c>
       <c r="C1" s="33">
         <f>([1]btc_ticker_price!$B$2/1000+8*3600)/86400+70*365+19</f>
-        <v>43235.578177546297</v>
+        <v>43237.736563101847</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
@@ -975,23 +974,23 @@
       </c>
       <c r="C5" s="7">
         <f>[1]usdt_c2c_price!$B$4</f>
-        <v>6.49</v>
+        <v>6.5</v>
       </c>
       <c r="D5" s="12">
         <f>B5/C5</f>
-        <v>15408.320493066256</v>
+        <v>15384.615384615385</v>
       </c>
       <c r="E5" s="12">
         <f>[1]btc_ticker_price!$B$4</f>
-        <v>8717.2900000000009</v>
+        <v>8285.5400000000009</v>
       </c>
       <c r="F5" s="21">
         <f>D5/E5</f>
-        <v>1.7675585523788075</v>
+        <v>1.856802982619767</v>
       </c>
       <c r="G5" s="14">
         <f>-($F$10/(F5)-1)</f>
-        <v>3.427420001195558E-3</v>
+        <v>2.1705787374365348E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1003,23 +1002,23 @@
         <v>100000</v>
       </c>
       <c r="C6" s="24">
-        <v>6.62</v>
+        <v>6.5</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" ref="D6:D10" si="0">B6/C6</f>
-        <v>15105.740181268882</v>
+        <v>15384.615384615385</v>
       </c>
       <c r="E6" s="12">
         <f>[1]btc_ticker_price!$C$4</f>
-        <v>8722.9490000000005</v>
+        <v>8292.8068999999996</v>
       </c>
       <c r="F6" s="21">
         <f t="shared" ref="F6:F10" si="1">D6/E6</f>
-        <v>1.7317240054101981</v>
+        <v>1.855175885575653</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" ref="G6:G7" si="2">-($F$10/(F6)-1)</f>
-        <v>-1.7194646109816247E-2</v>
+        <v>1.2954243574719859E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1031,23 +1030,23 @@
         <v>100000</v>
       </c>
       <c r="C7" s="25">
-        <v>6.6139999999999999</v>
+        <v>6.5679999999999996</v>
       </c>
       <c r="D7" s="12">
         <f t="shared" si="0"/>
-        <v>15119.443604475355</v>
+        <v>15225.334957369063</v>
       </c>
       <c r="E7" s="12">
         <f>[1]btc_ticker_price!$D$4</f>
-        <v>8711</v>
+        <v>8301.02</v>
       </c>
       <c r="F7" s="21">
         <f t="shared" si="1"/>
-        <v>1.7356725524595746</v>
+        <v>1.8341523038577261</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>-1.4880591587926872E-2</v>
+        <v>-1.0152014993080938E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1090,18 +1089,18 @@
       </c>
       <c r="C10" s="28">
         <f>[1]vhkd_c2c_price!$B$4</f>
-        <v>0.82199999999999995</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="D10" s="27">
         <f t="shared" si="0"/>
-        <v>121654.50121654502</v>
+        <v>121506.68286755773</v>
       </c>
       <c r="E10" s="15">
-        <v>69063</v>
+        <v>65581</v>
       </c>
       <c r="F10" s="29">
         <f t="shared" si="1"/>
-        <v>1.7615003868431001</v>
+        <v>1.8527726455460838</v>
       </c>
       <c r="G10" s="16"/>
     </row>
@@ -1157,23 +1156,23 @@
       </c>
       <c r="C16" s="12">
         <f>[1]btc_ticker_price!$B$3</f>
-        <v>8717.17</v>
+        <v>8283.7199999999993</v>
       </c>
       <c r="D16" s="12">
         <f>C16*B16</f>
-        <v>17434.34</v>
+        <v>16567.439999999999</v>
       </c>
       <c r="E16" s="12">
         <f>[1]usdt_c2c_price!$B$3</f>
-        <v>6.48</v>
+        <v>6.49</v>
       </c>
       <c r="F16" s="12">
         <f>D16*E16</f>
-        <v>112974.52320000001</v>
+        <v>107522.6856</v>
       </c>
       <c r="G16" s="14">
         <f>($F$21/(F16)-1)</f>
-        <v>-2.1180938252457371E-2</v>
+        <v>-2.1604663118645173E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1186,22 +1185,22 @@
       </c>
       <c r="C17" s="12">
         <f>[1]btc_ticker_price!$C$3</f>
-        <v>8718.7561999999998</v>
+        <v>8287.5108</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" ref="D17:D18" si="3">C17*B17</f>
-        <v>17437.5124</v>
+        <v>16575.0216</v>
       </c>
       <c r="E17" s="23">
-        <v>6.61</v>
+        <v>6.5</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" ref="F17:F18" si="4">D17*E17</f>
-        <v>115261.956964</v>
+        <v>107737.6404</v>
       </c>
       <c r="G17" s="14">
         <f t="shared" ref="G17:G18" si="5">($F$21/(F17)-1)</f>
-        <v>-4.0606113997021742E-2</v>
+        <v>-2.3556727162181379E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1214,22 +1213,22 @@
       </c>
       <c r="C18" s="12">
         <f>[1]btc_ticker_price!$D$3</f>
-        <v>8701.2999999999993</v>
+        <v>8300.7199999999993</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="3"/>
-        <v>17402.599999999999</v>
+        <v>16601.439999999999</v>
       </c>
       <c r="E18" s="23">
-        <v>6.61</v>
+        <v>6.4630000000000001</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="4"/>
-        <v>115031.186</v>
+        <v>107295.10672</v>
       </c>
       <c r="G18" s="14">
         <f t="shared" si="5"/>
-        <v>-3.8681416359560128E-2</v>
+        <v>-1.9529432273815095E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1271,19 +1270,19 @@
         <v>2</v>
       </c>
       <c r="C21" s="15">
-        <v>68582</v>
+        <v>65123</v>
       </c>
       <c r="D21" s="27">
         <f>C21*B21</f>
-        <v>137164</v>
+        <v>130246</v>
       </c>
       <c r="E21" s="28">
         <f>[1]vhkd_c2c_price!$B$3</f>
-        <v>0.80620000000000003</v>
+        <v>0.80769999999999997</v>
       </c>
       <c r="F21" s="27">
         <f>D21*E21</f>
-        <v>110581.6168</v>
+        <v>105199.6942</v>
       </c>
       <c r="G21" s="16"/>
     </row>
@@ -1354,11 +1353,11 @@
       </c>
       <c r="B1" s="32">
         <f>([1]btc_ticker_price!$B$2/1000+8*3600)/86400+70*365+19</f>
-        <v>43235.578177546297</v>
+        <v>43237.736563101847</v>
       </c>
       <c r="C1" s="33">
         <f>([1]btc_ticker_price!$B$2/1000+8*3600)/86400+70*365+19</f>
-        <v>43235.578177546297</v>
+        <v>43237.736563101847</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.25">
@@ -1413,23 +1412,23 @@
       </c>
       <c r="C5" s="7">
         <f>[1]usdt_c2c_price!$B$4</f>
-        <v>6.49</v>
+        <v>6.5</v>
       </c>
       <c r="D5" s="12">
         <f>B5/C5</f>
-        <v>15408.320493066256</v>
+        <v>15384.615384615385</v>
       </c>
       <c r="E5" s="20">
         <f>[1]eth_ticker_price!$B$4</f>
-        <v>733.01</v>
+        <v>704.38</v>
       </c>
       <c r="F5" s="13">
         <f>D5/E5</f>
-        <v>21.020614306852917</v>
+        <v>21.841357484050349</v>
       </c>
       <c r="G5" s="14">
         <f>-($F$10/(F5)-1)</f>
-        <v>9.7359321158936307E-3</v>
+        <v>1.0061462471344651E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1441,23 +1440,24 @@
         <v>100000</v>
       </c>
       <c r="C6" s="24">
-        <v>6.62</v>
+        <f>BTC!C6</f>
+        <v>6.5</v>
       </c>
       <c r="D6" s="12">
         <f t="shared" ref="D6:D10" si="0">B6/C6</f>
-        <v>15105.740181268882</v>
+        <v>15384.615384615385</v>
       </c>
       <c r="E6" s="20">
         <f>[1]eth_ticker_price!$C$4</f>
-        <v>733.7799</v>
+        <v>703.81910000000005</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" ref="F6:F10" si="1">D6/E6</f>
-        <v>20.586200550422383</v>
+        <v>21.858763686031516</v>
       </c>
       <c r="G6" s="14">
         <f t="shared" ref="G6:G7" si="2">-($F$10/(F6)-1)</f>
-        <v>-1.1160800748145627E-2</v>
+        <v>1.8016481815589236E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1469,23 +1469,24 @@
         <v>100000</v>
       </c>
       <c r="C7" s="25">
-        <v>6.6139999999999999</v>
+        <f>BTC!C7</f>
+        <v>6.5679999999999996</v>
       </c>
       <c r="D7" s="12">
         <f t="shared" si="0"/>
-        <v>15119.443604475355</v>
+        <v>15225.334957369063</v>
       </c>
       <c r="E7" s="20">
         <f>[1]eth_ticker_price!$D$4</f>
-        <v>734.15</v>
+        <v>704.71</v>
       </c>
       <c r="F7" s="13">
         <f t="shared" si="1"/>
-        <v>20.594488325921617</v>
+        <v>21.605107004823349</v>
       </c>
       <c r="G7" s="14">
         <f t="shared" si="2"/>
-        <v>-1.0753882470905696E-2</v>
+        <v>-9.9177883874523864E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1528,18 +1529,18 @@
       </c>
       <c r="C10" s="28">
         <f>[1]vhkd_c2c_price!$B$4</f>
-        <v>0.82199999999999995</v>
+        <v>0.82299999999999995</v>
       </c>
       <c r="D10" s="27">
         <f t="shared" si="0"/>
-        <v>121654.50121654502</v>
+        <v>121506.68286755773</v>
       </c>
       <c r="E10" s="15">
-        <v>5844.29</v>
+        <v>5568.75</v>
       </c>
       <c r="F10" s="30">
         <f t="shared" si="1"/>
-        <v>20.815959032927015</v>
+        <v>21.81938188418545</v>
       </c>
       <c r="G10" s="16"/>
     </row>
@@ -1598,23 +1599,23 @@
       </c>
       <c r="C16" s="20">
         <f>[1]eth_ticker_price!$B$3</f>
-        <v>733</v>
+        <v>704.1</v>
       </c>
       <c r="D16" s="12">
         <f>C16*B16</f>
-        <v>14660</v>
+        <v>14082</v>
       </c>
       <c r="E16" s="12">
         <f>[1]usdt_c2c_price!$B$3</f>
-        <v>6.48</v>
+        <v>6.49</v>
       </c>
       <c r="F16" s="12">
         <f>D16*E16</f>
-        <v>94996.800000000003</v>
+        <v>91392.180000000008</v>
       </c>
       <c r="G16" s="14">
         <f>($F$21/(F16)-1)</f>
-        <v>-1.6854355515133146E-2</v>
+        <v>-2.5494618029682781E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1627,22 +1628,23 @@
       </c>
       <c r="C17" s="20">
         <f>[1]eth_ticker_price!$C$3</f>
-        <v>732.327</v>
+        <v>702.86779999999999</v>
       </c>
       <c r="D17" s="12">
         <f t="shared" ref="D17:D18" si="3">C17*B17</f>
-        <v>14646.54</v>
+        <v>14057.356</v>
       </c>
       <c r="E17" s="23">
-        <v>6.61</v>
+        <f>BTC!E17</f>
+        <v>6.5</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" ref="F17:F18" si="4">D17*E17</f>
-        <v>96813.629400000005</v>
+        <v>91372.813999999998</v>
       </c>
       <c r="G17" s="14">
         <f t="shared" ref="G17:G18" si="5">($F$21/(F17)-1)</f>
-        <v>-3.5304318835918003E-2</v>
+        <v>-2.528807660449206E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1655,22 +1657,23 @@
       </c>
       <c r="C18" s="20">
         <f>[1]eth_ticker_price!$D$3</f>
-        <v>732.37</v>
+        <v>703.72</v>
       </c>
       <c r="D18" s="12">
         <f t="shared" si="3"/>
-        <v>14647.4</v>
+        <v>14074.400000000001</v>
       </c>
       <c r="E18" s="23">
-        <v>6.61</v>
+        <f>BTC!E18</f>
+        <v>6.4630000000000001</v>
       </c>
       <c r="F18" s="12">
         <f t="shared" si="4"/>
-        <v>96819.313999999998</v>
+        <v>90962.847200000004</v>
       </c>
       <c r="G18" s="14">
         <f t="shared" si="5"/>
-        <v>-3.5360959487897192E-2</v>
+        <v>-2.0895079458330912E-2</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1712,19 +1715,19 @@
         <v>20</v>
       </c>
       <c r="C21" s="15">
-        <v>5792.34</v>
+        <v>5513.32</v>
       </c>
       <c r="D21" s="27">
         <f>C21*B21</f>
-        <v>115846.8</v>
+        <v>110266.4</v>
       </c>
       <c r="E21" s="28">
         <f>[1]vhkd_c2c_price!$B$3</f>
-        <v>0.80620000000000003</v>
+        <v>0.80769999999999997</v>
       </c>
       <c r="F21" s="27">
         <f>D21*E21</f>
-        <v>93395.690159999998</v>
+        <v>89062.171279999995</v>
       </c>
       <c r="G21" s="16"/>
     </row>

</xml_diff>